<commit_message>
added edit form and verify form
</commit_message>
<xml_diff>
--- a/src/test/java/rc25/mFormsAutomation/TestData/AddResponse.xlsx
+++ b/src/test/java/rc25/mFormsAutomation/TestData/AddResponse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="540" windowWidth="18855" windowHeight="11190" activeTab="1"/>
+    <workbookView xWindow="150" yWindow="540" windowWidth="18855" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>vmidha@astegic.com</t>
   </si>
   <si>
-    <t>123456</t>
-  </si>
-  <si>
     <t>fluorodine OXYGEN white Fluoride Anticavity</t>
   </si>
   <si>
@@ -561,6 +558,9 @@
   </si>
   <si>
     <t>ol hydrochloride</t>
+  </si>
+  <si>
+    <t>Astegic1!</t>
   </si>
 </sst>
 </file>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1012,20 +1012,20 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1042,7 +1042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1060,43 +1060,43 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>21</v>
       </c>
       <c r="N1" s="18"/>
       <c r="O1" s="4"/>
@@ -1111,22 +1111,22 @@
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="D2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1141,22 +1141,22 @@
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -1171,22 +1171,22 @@
     </row>
     <row r="4" spans="1:23" ht="14.25">
       <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -1199,22 +1199,22 @@
     </row>
     <row r="5" spans="1:23" ht="14.25">
       <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -1227,22 +1227,22 @@
     </row>
     <row r="6" spans="1:23" ht="14.25">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -1255,26 +1255,26 @@
     </row>
     <row r="7" spans="1:23" ht="14.25">
       <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -1285,26 +1285,26 @@
     </row>
     <row r="8" spans="1:23" ht="14.25">
       <c r="A8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -1315,29 +1315,29 @@
     </row>
     <row r="9" spans="1:23" ht="14.25">
       <c r="A9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1347,29 +1347,29 @@
     </row>
     <row r="10" spans="1:23" ht="14.25">
       <c r="A10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1379,30 +1379,30 @@
     </row>
     <row r="11" spans="1:23" ht="14.25">
       <c r="A11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
@@ -1411,28 +1411,28 @@
     </row>
     <row r="12" spans="1:23" ht="14.25">
       <c r="A12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -1441,28 +1441,28 @@
     </row>
     <row r="13" spans="1:23" ht="14.25">
       <c r="A13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -1471,28 +1471,28 @@
     </row>
     <row r="14" spans="1:23" ht="14.25">
       <c r="A14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -1501,135 +1501,135 @@
     </row>
     <row r="15" spans="1:23" ht="14.25">
       <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="9"/>
       <c r="N15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="14.25">
       <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="9"/>
       <c r="N16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="9"/>
       <c r="N17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25">
       <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="9"/>
@@ -1637,22 +1637,22 @@
     </row>
     <row r="19" spans="1:14" ht="14.25">
       <c r="A19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -1660,13 +1660,13 @@
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="N19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1706,42 +1706,42 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1777,28 +1777,28 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>106</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -1822,19 +1822,19 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>175</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>176</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -1842,32 +1842,32 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>177</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>178</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1878,10 +1878,10 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1906,10 +1906,10 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1920,10 +1920,10 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1934,10 +1934,10 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1948,10 +1948,10 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1962,26 +1962,26 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1992,10 +1992,10 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2006,10 +2006,10 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2045,15 +2045,15 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2061,15 +2061,15 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2080,10 +2080,10 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2094,26 +2094,26 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2124,10 +2124,10 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2138,10 +2138,10 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2152,10 +2152,10 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -2166,10 +2166,10 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -2226,28 +2226,28 @@
   <sheetData>
     <row r="17" spans="1:14" ht="14.25">
       <c r="A17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -2256,28 +2256,28 @@
     </row>
     <row r="18" spans="1:14" ht="14.25">
       <c r="A18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -2286,28 +2286,28 @@
     </row>
     <row r="19" spans="1:14" ht="14.25">
       <c r="A19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
@@ -2316,31 +2316,31 @@
     </row>
     <row r="20" spans="1:14" ht="14.25">
       <c r="A20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>141</v>
-      </c>
       <c r="D20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="9"/>
@@ -2348,31 +2348,31 @@
     </row>
     <row r="21" spans="1:14" ht="14.25">
       <c r="A21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>148</v>
-      </c>
       <c r="D21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L21" s="10"/>
       <c r="M21" s="9"/>
@@ -2380,22 +2380,22 @@
     </row>
     <row r="22" spans="1:14" ht="14.25">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -2408,22 +2408,22 @@
     </row>
     <row r="23" spans="1:14" ht="14.25">
       <c r="A23" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="D23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>

</xml_diff>

<commit_message>
Changed the name of the files and updated view theme script
</commit_message>
<xml_diff>
--- a/src/test/java/rc25/mFormsAutomation/TestData/AddResponse.xlsx
+++ b/src/test/java/rc25/mFormsAutomation/TestData/AddResponse.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="540" windowWidth="18855" windowHeight="11190"/>
@@ -13,12 +13,12 @@
     <sheet name="Add Response" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="181">
   <si>
     <t>username</t>
   </si>
@@ -209,15 +209,9 @@
     <t>Hyperlink (Display only)</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>Treatment Set TS330156</t>
   </si>
   <si>
-    <t>Aug</t>
-  </si>
-  <si>
     <t>Dukal Corporation</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>Audio (Display only)</t>
   </si>
   <si>
-    <t>2015</t>
-  </si>
-  <si>
     <t>DawnMist Antiperspirant Deodorant</t>
   </si>
   <si>
@@ -251,9 +242,6 @@
     <t>Jun</t>
   </si>
   <si>
-    <t>2021</t>
-  </si>
-  <si>
     <t>topcare pain relief pm</t>
   </si>
   <si>
@@ -542,9 +530,6 @@
     <t>03:00</t>
   </si>
   <si>
-    <t>Nov</t>
-  </si>
-  <si>
     <t>2019</t>
   </si>
   <si>
@@ -557,10 +542,25 @@
     <t>14</t>
   </si>
   <si>
-    <t>ol hydrochloride</t>
-  </si>
-  <si>
     <t>Astegic1!</t>
+  </si>
+  <si>
+    <t>add form data</t>
+  </si>
+  <si>
+    <t>add response data</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>keshav vihar, jaipur</t>
+  </si>
+  <si>
+    <t>lorideinn</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,6 +602,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FF999999"/>
       </patternFill>
     </fill>
@@ -618,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -640,8 +646,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,7 +975,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1013,13 +1021,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>179</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>7</v>
@@ -1040,14 +1048,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
@@ -1095,10 +1104,10 @@
       <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="18"/>
+      <c r="N1" s="19"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="5"/>
@@ -1171,13 +1180,13 @@
     </row>
     <row r="4" spans="1:23" ht="14.25">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>24</v>
@@ -1186,26 +1195,26 @@
         <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="4"/>
       <c r="N4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>24</v>
@@ -1214,26 +1223,30 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>24</v>
@@ -1242,26 +1255,28 @@
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="4"/>
+      <c r="J6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
     <row r="7" spans="1:23" ht="14.25">
       <c r="A7" s="1" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>24</v>
@@ -1270,12 +1285,10 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="G7" s="8"/>
-      <c r="H7" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -1285,13 +1298,13 @@
     </row>
     <row r="8" spans="1:23" ht="14.25">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>24</v>
@@ -1300,28 +1313,26 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I8" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="8"/>
       <c r="M8" s="4"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="1:23" ht="14.25">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>24</v>
@@ -1330,363 +1341,28 @@
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="G9" s="8"/>
-      <c r="H9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="4"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:23" ht="14.25">
-      <c r="A10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:23" ht="14.25">
-      <c r="A11" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="I11" s="8"/>
-      <c r="J11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-    </row>
-    <row r="12" spans="1:23" ht="14.25">
-      <c r="A12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:23" ht="14.25">
-      <c r="A13" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="1:23" ht="14.25">
-      <c r="A14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-    </row>
-    <row r="15" spans="1:23" ht="14.25">
-      <c r="A15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="14.25">
-      <c r="A16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="14.25">
-      <c r="A17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="14.25">
-      <c r="A18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L18" s="10"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="1:14" ht="14.25">
-      <c r="A19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="M1:N1"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" sqref="D2:E19">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" sqref="D2:E9">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H7:H10">
-      <formula1>"'1,'2,'3,'4,'5,'6,'7,'8,'9,'10"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I10">
-      <formula1>"'60,'90,'120,'150,'180,'210,'240,'270,'300"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I9">
-      <formula1>"'60,'90,'120,'150,'180"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H11">
+    <dataValidation type="list" allowBlank="1" sqref="H5">
       <formula1>"Number,Smiley,Star"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1699,7 +1375,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1725,23 +1401,23 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>72</v>
+      <c r="A2" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1762,16 +1438,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA26"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="99.42578125" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1780,25 +1456,25 @@
         <v>10</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>109</v>
-      </c>
       <c r="H1" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -1828,13 +1504,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>174</v>
-      </c>
       <c r="E2" s="16" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -1845,26 +1521,26 @@
         <v>28</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>137</v>
@@ -1878,24 +1554,26 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="15" t="s">
+        <v>69</v>
+      </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1906,10 +1584,10 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1920,24 +1598,26 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="20" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>161</v>
+        <v>110</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>160</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1946,259 +1626,13 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A14" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A15" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A21" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A25" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" sqref="F20 F3">
+    <dataValidation type="list" allowBlank="1" sqref="G5">
+      <formula1>"'1,'2,'3,'4,'5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F3">
       <formula1>"'00:00,'01:00,'02:00,'03:00,'04:00,'05:00,'06:00,'07:00,'08:00,'09:00,'10:00,'11:00,'12:00,'13:00,'14:00,'15:00,'16:00,'17:00,'18:00,'19:00,'20:00,'21:00,'22:00,'23:00"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G11">
-      <formula1>"'1,'2,'3,'4,'5"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="E2:E3">
       <formula1>"'2015,'2016,'2017,'2018,'2019,'2020,'2021,'2022,'2023,'2024,'2025"</formula1>
@@ -2216,23 +1650,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A17:N23"/>
+  <dimension ref="A17:N83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD16"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="17" spans="1:14" ht="14.25">
       <c r="A17" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>24</v>
@@ -2241,7 +1675,7 @@
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -2256,13 +1690,13 @@
     </row>
     <row r="18" spans="1:14" ht="14.25">
       <c r="A18" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>24</v>
@@ -2271,7 +1705,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -2286,13 +1720,13 @@
     </row>
     <row r="19" spans="1:14" ht="14.25">
       <c r="A19" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>24</v>
@@ -2301,7 +1735,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -2316,22 +1750,22 @@
     </row>
     <row r="20" spans="1:14" ht="14.25">
       <c r="A20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -2348,13 +1782,13 @@
     </row>
     <row r="21" spans="1:14" ht="14.25">
       <c r="A21" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>24</v>
@@ -2363,7 +1797,7 @@
         <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -2380,13 +1814,13 @@
     </row>
     <row r="22" spans="1:14" ht="14.25">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>24</v>
@@ -2395,7 +1829,7 @@
         <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -2408,13 +1842,13 @@
     </row>
     <row r="23" spans="1:14" ht="14.25">
       <c r="A23" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>24</v>
@@ -2423,7 +1857,7 @@
         <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -2434,10 +1868,600 @@
       <c r="M23" s="4"/>
       <c r="N23" s="9"/>
     </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A35" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A36" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A37" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A38" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A39" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A40" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A41" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="14.25">
+      <c r="A52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G52" s="8"/>
+      <c r="H52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="9"/>
+    </row>
+    <row r="53" spans="1:14" ht="14.25">
+      <c r="A53" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G53" s="8"/>
+      <c r="H53" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="9"/>
+    </row>
+    <row r="54" spans="1:14" ht="14.25">
+      <c r="A54" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G54" s="8"/>
+      <c r="H54" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="9"/>
+    </row>
+    <row r="55" spans="1:14" ht="14.25">
+      <c r="A55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G55" s="8"/>
+      <c r="H55" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="9"/>
+    </row>
+    <row r="59" spans="1:14" ht="14.25">
+      <c r="A59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+    </row>
+    <row r="60" spans="1:14" ht="14.25">
+      <c r="A60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="14.25">
+      <c r="A61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="14.25">
+      <c r="A62" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="14.25">
+      <c r="A63" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L63" s="10"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+    </row>
+    <row r="64" spans="1:14" ht="14.25">
+      <c r="A64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A71" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A72" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A73" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A74" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A78" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A79" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A80" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A81" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A82" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A83" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D17:E23">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" sqref="D17:E23 D59:E64 D52:E55">
       <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="F40">
+      <formula1>"'00:00,'01:00,'02:00,'03:00,'04:00,'05:00,'06:00,'07:00,'08:00,'09:00,'10:00,'11:00,'12:00,'13:00,'14:00,'15:00,'16:00,'17:00,'18:00,'19:00,'20:00,'21:00,'22:00,'23:00"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="I54">
+      <formula1>"'60,'90,'120,'150,'180"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="I55">
+      <formula1>"'60,'90,'120,'150,'180,'210,'240,'270,'300"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="H52:H55">
+      <formula1>"'1,'2,'3,'4,'5,'6,'7,'8,'9,'10"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>